<commit_message>
add marker set template
</commit_message>
<xml_diff>
--- a/server/marker-template/Marker_Template.xlsx
+++ b/server/marker-template/Marker_Template.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
-    <sheet name="marker_template" sheetId="1" r:id="rId1"/>
+    <sheet name="marker_set_template" sheetId="2" r:id="rId1"/>
+    <sheet name="marker_template" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>id</t>
   </si>
@@ -32,9 +33,6 @@
     <t>A</t>
   </si>
   <si>
-    <t>marker_template</t>
-  </si>
-  <si>
     <t>marker_name</t>
   </si>
   <si>
@@ -102,6 +100,12 @@
   </si>
   <si>
     <t>{"shape":"fault","dashArray":[5,5]}</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>id_marker_template</t>
   </si>
 </sst>
 </file>
@@ -432,10 +436,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,39 +489,39 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" s="1">
         <v>1</v>
@@ -497,17 +532,17 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
+      <c r="B3" s="1">
+        <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F3" s="1">
         <v>1</v>
@@ -517,17 +552,17 @@
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
+      <c r="B4" s="1">
+        <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" s="1">
         <v>1</v>
@@ -537,17 +572,17 @@
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
+      <c r="B5" s="1">
+        <v>1</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="1">
         <v>1</v>
@@ -557,17 +592,17 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>11</v>
+      <c r="B6" s="1">
+        <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6" s="1">
         <v>1</v>
@@ -577,17 +612,17 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>11</v>
+      <c r="B7" s="1">
+        <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
         <v>18</v>
       </c>
-      <c r="D7" t="s">
-        <v>19</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F7" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
marker default lineWidth = 2
</commit_message>
<xml_diff>
--- a/server/marker-template/Marker_Template.xlsx
+++ b/server/marker-template/Marker_Template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\wi-backend\server\marker-template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\wi-backend\server\marker-template\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20937AAD-B1CA-478C-AADB-0F316D6CAC00}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="marker_set_template" sheetId="2" r:id="rId1"/>
@@ -114,7 +115,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -438,7 +439,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -469,11 +470,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,7 +532,7 @@
         <v>19</v>
       </c>
       <c r="F2" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G2" s="1">
         <v>1</v>
@@ -555,7 +556,7 @@
         <v>20</v>
       </c>
       <c r="F3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G3" s="1">
         <v>2</v>
@@ -578,7 +579,7 @@
         <v>21</v>
       </c>
       <c r="F4" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G4" s="1">
         <v>3</v>
@@ -601,7 +602,7 @@
         <v>22</v>
       </c>
       <c r="F5" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G5" s="1">
         <v>4</v>
@@ -624,7 +625,7 @@
         <v>23</v>
       </c>
       <c r="F6" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G6" s="1">
         <v>5</v>
@@ -647,7 +648,7 @@
         <v>24</v>
       </c>
       <c r="F7" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G7" s="1">
         <v>6</v>

</xml_diff>